<commit_message>
added readings for plotting
</commit_message>
<xml_diff>
--- a/Semester8/lab/exp4/exp4- thermoelectric.xlsx
+++ b/Semester8/lab/exp4/exp4- thermoelectric.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -200,7 +200,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -476,11 +475,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1324267648"/>
-        <c:axId val="-1324259488"/>
+        <c:axId val="1665368160"/>
+        <c:axId val="1665376320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1324267648"/>
+        <c:axId val="1665368160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -537,12 +536,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1324259488"/>
+        <c:crossAx val="1665376320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1324259488"/>
+        <c:axId val="1665376320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -599,7 +598,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1324267648"/>
+        <c:crossAx val="1665368160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1119,11 +1118,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1324265472"/>
-        <c:axId val="-1324264928"/>
+        <c:axId val="1665375232"/>
+        <c:axId val="1665371424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1324265472"/>
+        <c:axId val="1665375232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1180,12 +1179,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1324264928"/>
+        <c:crossAx val="1665371424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1324264928"/>
+        <c:axId val="1665371424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1242,7 +1241,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1324265472"/>
+        <c:crossAx val="1665375232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1715,11 +1714,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-1324257312"/>
-        <c:axId val="-1326521312"/>
+        <c:axId val="1665369248"/>
+        <c:axId val="1665365440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-1324257312"/>
+        <c:axId val="1665369248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1776,12 +1775,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1326521312"/>
+        <c:crossAx val="1665365440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-1326521312"/>
+        <c:axId val="1665365440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1838,7 +1837,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1324257312"/>
+        <c:crossAx val="1665369248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2304,11 +2303,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-841412192"/>
-        <c:axId val="-841420896"/>
+        <c:axId val="1665376864"/>
+        <c:axId val="1665373056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-841412192"/>
+        <c:axId val="1665376864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2365,12 +2364,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-841420896"/>
+        <c:crossAx val="1665373056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-841420896"/>
+        <c:axId val="1665373056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2427,7 +2426,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-841412192"/>
+        <c:crossAx val="1665376864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5366,7 +5365,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView topLeftCell="E25" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:F52"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6882,8 +6883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6913,7 +6914,7 @@
         <v>-0.7</v>
       </c>
       <c r="D2">
-        <f>B2-C2</f>
+        <f t="shared" ref="D2:D43" si="0">B2-C2</f>
         <v>24.7</v>
       </c>
       <c r="E2">
@@ -6928,7 +6929,7 @@
         <v>-0.7</v>
       </c>
       <c r="D3">
-        <f>B3-C3</f>
+        <f t="shared" si="0"/>
         <v>24.7</v>
       </c>
       <c r="E3">
@@ -6943,7 +6944,7 @@
         <v>-0.7</v>
       </c>
       <c r="D4">
-        <f>B4-C4</f>
+        <f t="shared" si="0"/>
         <v>25.7</v>
       </c>
       <c r="E4">
@@ -6958,7 +6959,7 @@
         <v>-0.7</v>
       </c>
       <c r="D5">
-        <f>B5-C5</f>
+        <f t="shared" si="0"/>
         <v>27.7</v>
       </c>
       <c r="E5">
@@ -6973,7 +6974,7 @@
         <v>-0.7</v>
       </c>
       <c r="D6">
-        <f>B6-C6</f>
+        <f t="shared" si="0"/>
         <v>29.7</v>
       </c>
       <c r="E6">
@@ -6988,7 +6989,7 @@
         <v>-0.7</v>
       </c>
       <c r="D7">
-        <f>B7-C7</f>
+        <f t="shared" si="0"/>
         <v>31.7</v>
       </c>
       <c r="E7">
@@ -7003,7 +7004,7 @@
         <v>-0.7</v>
       </c>
       <c r="D8">
-        <f>B8-C8</f>
+        <f t="shared" si="0"/>
         <v>33.700000000000003</v>
       </c>
       <c r="E8">
@@ -7018,7 +7019,7 @@
         <v>-0.7</v>
       </c>
       <c r="D9">
-        <f>B9-C9</f>
+        <f t="shared" si="0"/>
         <v>36.700000000000003</v>
       </c>
       <c r="E9">
@@ -7033,7 +7034,7 @@
         <v>-0.7</v>
       </c>
       <c r="D10">
-        <f>B10-C10</f>
+        <f t="shared" si="0"/>
         <v>39.700000000000003</v>
       </c>
       <c r="E10">
@@ -7048,7 +7049,7 @@
         <v>-0.7</v>
       </c>
       <c r="D11">
-        <f>B11-C11</f>
+        <f t="shared" si="0"/>
         <v>41.7</v>
       </c>
       <c r="E11">
@@ -7063,7 +7064,7 @@
         <v>-0.7</v>
       </c>
       <c r="D12">
-        <f>B12-C12</f>
+        <f t="shared" si="0"/>
         <v>43.7</v>
       </c>
       <c r="E12">
@@ -7078,7 +7079,7 @@
         <v>-0.7</v>
       </c>
       <c r="D13">
-        <f>B13-C13</f>
+        <f t="shared" si="0"/>
         <v>46.7</v>
       </c>
       <c r="E13">
@@ -7093,7 +7094,7 @@
         <v>-0.7</v>
       </c>
       <c r="D14">
-        <f>B14-C14</f>
+        <f t="shared" si="0"/>
         <v>49.7</v>
       </c>
       <c r="E14">
@@ -7108,7 +7109,7 @@
         <v>-0.7</v>
       </c>
       <c r="D15">
-        <f>B15-C15</f>
+        <f t="shared" si="0"/>
         <v>51.7</v>
       </c>
       <c r="E15">
@@ -7123,7 +7124,7 @@
         <v>-0.7</v>
       </c>
       <c r="D16">
-        <f>B16-C16</f>
+        <f t="shared" si="0"/>
         <v>53.7</v>
       </c>
       <c r="E16">
@@ -7138,7 +7139,7 @@
         <v>-0.7</v>
       </c>
       <c r="D17">
-        <f>B17-C17</f>
+        <f t="shared" si="0"/>
         <v>56.7</v>
       </c>
       <c r="E17">
@@ -7153,7 +7154,7 @@
         <v>-0.7</v>
       </c>
       <c r="D18">
-        <f>B18-C18</f>
+        <f t="shared" si="0"/>
         <v>58.7</v>
       </c>
       <c r="E18">
@@ -7168,7 +7169,7 @@
         <v>-0.7</v>
       </c>
       <c r="D19">
-        <f>B19-C19</f>
+        <f t="shared" si="0"/>
         <v>61.7</v>
       </c>
       <c r="E19">
@@ -7183,7 +7184,7 @@
         <v>-0.7</v>
       </c>
       <c r="D20">
-        <f>B20-C20</f>
+        <f t="shared" si="0"/>
         <v>63.7</v>
       </c>
       <c r="E20">
@@ -7198,7 +7199,7 @@
         <v>-0.7</v>
       </c>
       <c r="D21">
-        <f>B21-C21</f>
+        <f t="shared" si="0"/>
         <v>65.7</v>
       </c>
       <c r="E21">
@@ -7213,7 +7214,7 @@
         <v>-0.7</v>
       </c>
       <c r="D22">
-        <f>B22-C22</f>
+        <f t="shared" si="0"/>
         <v>68.7</v>
       </c>
       <c r="E22">
@@ -7228,7 +7229,7 @@
         <v>-0.7</v>
       </c>
       <c r="D23">
-        <f>B23-C23</f>
+        <f t="shared" si="0"/>
         <v>70.7</v>
       </c>
       <c r="E23">
@@ -7243,7 +7244,7 @@
         <v>-0.7</v>
       </c>
       <c r="D24">
-        <f>B24-C24</f>
+        <f t="shared" si="0"/>
         <v>73.7</v>
       </c>
       <c r="E24">
@@ -7258,7 +7259,7 @@
         <v>-0.7</v>
       </c>
       <c r="D25">
-        <f>B25-C25</f>
+        <f t="shared" si="0"/>
         <v>75.7</v>
       </c>
       <c r="E25">
@@ -7273,7 +7274,7 @@
         <v>-0.7</v>
       </c>
       <c r="D26">
-        <f>B26-C26</f>
+        <f t="shared" si="0"/>
         <v>78.7</v>
       </c>
       <c r="E26">
@@ -7288,7 +7289,7 @@
         <v>-0.7</v>
       </c>
       <c r="D27">
-        <f>B27-C27</f>
+        <f t="shared" si="0"/>
         <v>80.7</v>
       </c>
       <c r="E27">
@@ -7303,7 +7304,7 @@
         <v>-0.7</v>
       </c>
       <c r="D28">
-        <f>B28-C28</f>
+        <f t="shared" si="0"/>
         <v>82.7</v>
       </c>
       <c r="E28">
@@ -7318,7 +7319,7 @@
         <v>-0.7</v>
       </c>
       <c r="D29">
-        <f>B29-C29</f>
+        <f t="shared" si="0"/>
         <v>85.7</v>
       </c>
       <c r="E29">
@@ -7333,7 +7334,7 @@
         <v>-0.7</v>
       </c>
       <c r="D30">
-        <f>B30-C30</f>
+        <f t="shared" si="0"/>
         <v>87.7</v>
       </c>
       <c r="E30">
@@ -7348,7 +7349,7 @@
         <v>-0.7</v>
       </c>
       <c r="D31">
-        <f>B31-C31</f>
+        <f t="shared" si="0"/>
         <v>89.7</v>
       </c>
       <c r="E31">
@@ -7363,7 +7364,7 @@
         <v>-0.7</v>
       </c>
       <c r="D32">
-        <f>B32-C32</f>
+        <f t="shared" si="0"/>
         <v>92.7</v>
       </c>
       <c r="E32">
@@ -7378,7 +7379,7 @@
         <v>-0.7</v>
       </c>
       <c r="D33">
-        <f>B33-C33</f>
+        <f t="shared" si="0"/>
         <v>95.7</v>
       </c>
       <c r="E33">
@@ -7393,7 +7394,7 @@
         <v>-0.7</v>
       </c>
       <c r="D34">
-        <f>B34-C34</f>
+        <f t="shared" si="0"/>
         <v>98.7</v>
       </c>
       <c r="E34">
@@ -7408,7 +7409,7 @@
         <v>-0.7</v>
       </c>
       <c r="D35">
-        <f>B35-C35</f>
+        <f t="shared" si="0"/>
         <v>102.7</v>
       </c>
       <c r="E35">
@@ -7426,7 +7427,7 @@
         <v>-0.7</v>
       </c>
       <c r="D36">
-        <f>B36-C36</f>
+        <f t="shared" si="0"/>
         <v>105.7</v>
       </c>
       <c r="E36">
@@ -7441,7 +7442,7 @@
         <v>-0.7</v>
       </c>
       <c r="D37">
-        <f>B37-C37</f>
+        <f t="shared" si="0"/>
         <v>108.7</v>
       </c>
       <c r="E37">
@@ -7456,7 +7457,7 @@
         <v>-0.7</v>
       </c>
       <c r="D38">
-        <f>B38-C38</f>
+        <f t="shared" si="0"/>
         <v>110.7</v>
       </c>
       <c r="E38">
@@ -7471,7 +7472,7 @@
         <v>-0.7</v>
       </c>
       <c r="D39">
-        <f>B39-C39</f>
+        <f t="shared" si="0"/>
         <v>112.7</v>
       </c>
       <c r="E39">
@@ -7486,7 +7487,7 @@
         <v>-0.7</v>
       </c>
       <c r="D40">
-        <f>B40-C40</f>
+        <f t="shared" si="0"/>
         <v>114.7</v>
       </c>
       <c r="E40">
@@ -7501,7 +7502,7 @@
         <v>-0.7</v>
       </c>
       <c r="D41">
-        <f>B41-C41</f>
+        <f t="shared" si="0"/>
         <v>116.7</v>
       </c>
       <c r="E41">
@@ -7516,7 +7517,7 @@
         <v>-0.7</v>
       </c>
       <c r="D42">
-        <f>B42-C42</f>
+        <f t="shared" si="0"/>
         <v>118.7</v>
       </c>
       <c r="E42">
@@ -7531,7 +7532,7 @@
         <v>-0.7</v>
       </c>
       <c r="D43">
-        <f>B43-C43</f>
+        <f t="shared" si="0"/>
         <v>120.7</v>
       </c>
       <c r="E43">

</xml_diff>